<commit_message>
Exploring FMP's stock price data; sticking to yf
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/NVDA/annual/stock_price_data.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/NVDA/annual/stock_price_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>high</t>
   </si>
@@ -26,48 +26,6 @@
   </si>
   <si>
     <t>index</t>
-  </si>
-  <si>
-    <t>NVDA-FY-1999</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2000</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2001</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2002</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2003</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2004</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2005</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2006</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2007</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2008</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2009</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2010</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2011</t>
-  </si>
-  <si>
-    <t>NVDA-FY-2012</t>
   </si>
   <si>
     <t>NVDA-FY-2013</t>
@@ -455,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,13 +443,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.005208015441895</v>
+        <v>4.110000133514404</v>
       </c>
       <c r="C3">
-        <v>0.3333329856395721</v>
+        <v>3.009999990463257</v>
       </c>
       <c r="D3">
-        <v>0.5189965349577722</v>
+        <v>3.605458164595038</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -499,13 +457,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>3.666666984558105</v>
+        <v>5.3125</v>
       </c>
       <c r="C4">
-        <v>0.7291669845581055</v>
+        <v>3.829999923706055</v>
       </c>
       <c r="D4">
-        <v>2.272824106463398</v>
+        <v>4.699183270275831</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -513,13 +471,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>6.054999828338623</v>
+        <v>8.484999656677246</v>
       </c>
       <c r="C5">
-        <v>1.666666984558105</v>
+        <v>4.735000133514404</v>
       </c>
       <c r="D5">
-        <v>3.545779787577116</v>
+        <v>6.087988281622529</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -527,13 +485,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>5.695833206176758</v>
+        <v>29.98250007629395</v>
       </c>
       <c r="C6">
-        <v>0.6000000238418579</v>
+        <v>6.1875</v>
       </c>
       <c r="D6">
-        <v>2.105551130268204</v>
+        <v>14.82492032374044</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -541,13 +499,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.3125</v>
+        <v>60.83499908447266</v>
       </c>
       <c r="C7">
-        <v>0.7774999737739563</v>
+        <v>23.79249954223633</v>
       </c>
       <c r="D7">
-        <v>1.547145161777735</v>
+        <v>39.58842625560988</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -555,13 +513,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.27916693687439</v>
+        <v>73.19000244140625</v>
       </c>
       <c r="C8">
-        <v>0.7749999761581421</v>
+        <v>31.11499977111816</v>
       </c>
       <c r="D8">
-        <v>1.60138114111357</v>
+        <v>56.77958995819092</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -569,13 +527,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>3.896667003631592</v>
+        <v>64.875</v>
       </c>
       <c r="C9">
-        <v>1.743332982063293</v>
+        <v>32.75</v>
       </c>
       <c r="D9">
-        <v>2.505431586527729</v>
+        <v>45.24611545273982</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -583,13 +541,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>6.493332862854004</v>
+        <v>147.2675018310547</v>
       </c>
       <c r="C10">
-        <v>2.861666917800903</v>
+        <v>45.16999816894531</v>
       </c>
       <c r="D10">
-        <v>4.666273349761963</v>
+        <v>103.7769730389118</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -597,208 +555,12 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>9.917499542236328</v>
+        <v>346.4700012207031</v>
       </c>
       <c r="C11">
-        <v>4.673333168029785</v>
+        <v>115.6650009155273</v>
       </c>
       <c r="D11">
-        <v>7.001689627414613</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>6.897500038146973</v>
-      </c>
-      <c r="C12">
-        <v>1.4375</v>
-      </c>
-      <c r="D12">
-        <v>3.616511867922756</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>4.739999771118164</v>
-      </c>
-      <c r="C13">
-        <v>1.802500009536743</v>
-      </c>
-      <c r="D13">
-        <v>3.143864534290663</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>6.262499809265137</v>
-      </c>
-      <c r="C14">
-        <v>2.162499904632568</v>
-      </c>
-      <c r="D14">
-        <v>3.469593245831747</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>6.542500019073486</v>
-      </c>
-      <c r="C15">
-        <v>2.867500066757202</v>
-      </c>
-      <c r="D15">
-        <v>4.087320708658591</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>4.224999904632568</v>
-      </c>
-      <c r="C16">
-        <v>2.787499904632568</v>
-      </c>
-      <c r="D16">
-        <v>3.341757016967099</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>4.110000133514404</v>
-      </c>
-      <c r="C17">
-        <v>3.009999990463257</v>
-      </c>
-      <c r="D17">
-        <v>3.605458164595038</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>5.3125</v>
-      </c>
-      <c r="C18">
-        <v>3.829999923706055</v>
-      </c>
-      <c r="D18">
-        <v>4.699183270275831</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>8.484999656677246</v>
-      </c>
-      <c r="C19">
-        <v>4.735000133514404</v>
-      </c>
-      <c r="D19">
-        <v>6.087988281622529</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>29.98250007629395</v>
-      </c>
-      <c r="C20">
-        <v>6.1875</v>
-      </c>
-      <c r="D20">
-        <v>14.82492032374044</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>60.83499908447266</v>
-      </c>
-      <c r="C21">
-        <v>23.79249954223633</v>
-      </c>
-      <c r="D21">
-        <v>39.58842625560988</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>73.19000244140625</v>
-      </c>
-      <c r="C22">
-        <v>31.11499977111816</v>
-      </c>
-      <c r="D22">
-        <v>56.77958995819092</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>64.875</v>
-      </c>
-      <c r="C23">
-        <v>32.75</v>
-      </c>
-      <c r="D23">
-        <v>45.24611545273982</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>147.2675018310547</v>
-      </c>
-      <c r="C24">
-        <v>45.16999816894531</v>
-      </c>
-      <c r="D24">
-        <v>103.7769730389118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>346.4700012207031</v>
-      </c>
-      <c r="C25">
-        <v>115.6650009155273</v>
-      </c>
-      <c r="D25">
         <v>204.6822222149561</v>
       </c>
     </row>

</xml_diff>